<commit_message>
correcciones a las tablas
</commit_message>
<xml_diff>
--- a/latamReturns&Ratios/latamIndustryRatios.xlsx
+++ b/latamReturns&Ratios/latamIndustryRatios.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,16 +28,567 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <color rgb="00F1F1F1"/>
+    </font>
+    <font>
+      <color rgb="00000000"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="111">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F5E4D5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F6E7DF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F1D1EC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D0EBFE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D3CBFB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EBECF0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EFD0EA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DCF5F8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CDF3EF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D5D0CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F6FAF1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EFEEF9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DDE6EB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FDFAD4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D5DBDF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFE1E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CFE7E4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E9DFC9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E7CBFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F8FCE0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DECDD9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DEFED2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D3F1D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EDFEE4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E6D6F6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E8FDF3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F2FDEB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F7E2EC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DECFFE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F0D5D1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C8D0F7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E6DCF7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E1D1FB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EEE6D0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CCEEC9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D5FFF5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F1F1EA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DDFEC9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D7E9FB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FDEEFB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E1DFE0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FEFAD1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E9E2D0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E6DBD8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FDCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E4C9E7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DED8E9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ED5F3C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0078C565"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0036A657"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0084CA66"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="007FC866"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F57748"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F7844E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0073C264"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005DB961"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F88C51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F88950"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0051B35E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0070C164"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0063BC62"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004BB05C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0054B45F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00128A49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="001B9950"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F67F4B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="000F8446"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E75337"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E95538"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EE613E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F8864F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E54E35"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F57547"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E65036"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00006837"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00108647"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0045AD5B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00279F53"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002DA155"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="007DC765"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F7814C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EB5A3A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F46D43"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00199750"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0042AC5A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0069BE63"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005AB760"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0057B65F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00219C52"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0039A758"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="003FAA59"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="007AC665"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00138C4A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="001E9A51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="000E8245"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DB382B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F57245"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0048AE5C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0075C465"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="006EC064"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0066BD63"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0082C966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DE402E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EF633F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CE2827"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CA2427"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A50026"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F67C4A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C62027"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -51,36 +602,124 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="49" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="50" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="51" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="52" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="53" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="54" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="55" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="56" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="57" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="58" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="59" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="60" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="61" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="62" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="63" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="64" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="65" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="66" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="67" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="68" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="69" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="70" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="71" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="72" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="73" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="74" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="75" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="76" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="77" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="78" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="79" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="80" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="81" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="82" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="83" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="84" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="85" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="86" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="87" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="88" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="89" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="90" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="91" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="92" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="93" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="94" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="95" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="96" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="97" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="98" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="99" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="100" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="101" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="102" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="103" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="104" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="105" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="106" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="107" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="108" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="109" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="110" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -477,12 +1116,12 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Consumer Staples</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>ABEV</t>
         </is>
@@ -492,13 +1131,17 @@
           <t>ABEV/KOF</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="3" t="n">
         <v>-2.57</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n"/>
-      <c r="B3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Consumer Staples</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
         <is>
           <t>ASAI</t>
         </is>
@@ -508,13 +1151,17 @@
           <t>ASAI/ABEV</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="5" t="n">
         <v>2.18</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n"/>
-      <c r="B4" s="1" t="inlineStr">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Consumer Staples</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
         <is>
           <t>ASAI</t>
         </is>
@@ -524,13 +1171,17 @@
           <t>ASAI/CCU</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="5" t="n">
         <v>2.18</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n"/>
-      <c r="B5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Consumer Staples</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>ASAI</t>
         </is>
@@ -540,13 +1191,17 @@
           <t>ASAI/EXTO</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" s="6" t="n">
         <v>2.88</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n"/>
-      <c r="B6" s="1" t="inlineStr">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Consumer Staples</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="inlineStr">
         <is>
           <t>BRFS</t>
         </is>
@@ -556,13 +1211,17 @@
           <t>BRFS/EXTO</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="8" t="n">
         <v>2.03</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n"/>
-      <c r="B7" s="1" t="inlineStr">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Consumer Staples</t>
+        </is>
+      </c>
+      <c r="B7" s="9" t="inlineStr">
         <is>
           <t>CRESY</t>
         </is>
@@ -572,13 +1231,17 @@
           <t>CRESY/EXTO</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="10" t="n">
         <v>2.08</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n"/>
-      <c r="B8" s="1" t="inlineStr">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Consumer Staples</t>
+        </is>
+      </c>
+      <c r="B8" s="11" t="inlineStr">
         <is>
           <t>EXTO</t>
         </is>
@@ -588,13 +1251,17 @@
           <t>EXTO/ASAI</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" s="12" t="n">
         <v>-2.26</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n"/>
-      <c r="B9" s="1" t="inlineStr">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Consumer Staples</t>
+        </is>
+      </c>
+      <c r="B9" s="11" t="inlineStr">
         <is>
           <t>EXTO</t>
         </is>
@@ -604,13 +1271,17 @@
           <t>EXTO/KOF</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" s="13" t="n">
         <v>-2.12</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n"/>
-      <c r="B10" s="1" t="inlineStr">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Consumer Staples</t>
+        </is>
+      </c>
+      <c r="B10" s="14" t="inlineStr">
         <is>
           <t>KOF</t>
         </is>
@@ -620,13 +1291,17 @@
           <t>KOF/ABEV</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" s="6" t="n">
         <v>2.88</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n"/>
-      <c r="B11" s="1" t="inlineStr">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Consumer Staples</t>
+        </is>
+      </c>
+      <c r="B11" s="14" t="inlineStr">
         <is>
           <t>KOF</t>
         </is>
@@ -636,13 +1311,17 @@
           <t>KOF/CCU</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="D11" s="15" t="n">
         <v>2.24</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n"/>
-      <c r="B12" s="1" t="inlineStr">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Consumer Staples</t>
+        </is>
+      </c>
+      <c r="B12" s="14" t="inlineStr">
         <is>
           <t>KOF</t>
         </is>
@@ -652,17 +1331,17 @@
           <t>KOF/EXTO</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="D12" s="16" t="n">
         <v>2.49</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+      <c r="A13" t="inlineStr">
         <is>
           <t>Energy</t>
         </is>
       </c>
-      <c r="B13" s="1" t="inlineStr">
+      <c r="B13" s="17" t="inlineStr">
         <is>
           <t>CSAN</t>
         </is>
@@ -672,13 +1351,17 @@
           <t>CSAN/YPF</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D13" s="18" t="n">
         <v>-2.01</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n"/>
-      <c r="B14" s="1" t="inlineStr">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Energy</t>
+        </is>
+      </c>
+      <c r="B14" s="17" t="inlineStr">
         <is>
           <t>CSAN</t>
         </is>
@@ -688,13 +1371,17 @@
           <t>CSAN/VIST</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" s="19" t="n">
         <v>-2.04</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n"/>
-      <c r="B15" s="1" t="inlineStr">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Energy</t>
+        </is>
+      </c>
+      <c r="B15" s="17" t="inlineStr">
         <is>
           <t>CSAN</t>
         </is>
@@ -704,13 +1391,17 @@
           <t>CSAN/UGP</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="D15" s="19" t="n">
         <v>-2.05</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n"/>
-      <c r="B16" s="1" t="inlineStr">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Energy</t>
+        </is>
+      </c>
+      <c r="B16" s="20" t="inlineStr">
         <is>
           <t>PBR</t>
         </is>
@@ -720,13 +1411,17 @@
           <t>PBR/CSAN</t>
         </is>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" s="8" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n"/>
-      <c r="B17" s="1" t="inlineStr">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Energy</t>
+        </is>
+      </c>
+      <c r="B17" s="21" t="inlineStr">
         <is>
           <t>UGP</t>
         </is>
@@ -736,13 +1431,17 @@
           <t>UGP/CSAN</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="D17" s="22" t="n">
         <v>2.61</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n"/>
-      <c r="B18" s="1" t="inlineStr">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Energy</t>
+        </is>
+      </c>
+      <c r="B18" s="21" t="inlineStr">
         <is>
           <t>UGP</t>
         </is>
@@ -752,13 +1451,17 @@
           <t>UGP/EC</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="D18" s="23" t="n">
         <v>2.26</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n"/>
-      <c r="B19" s="1" t="inlineStr">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Energy</t>
+        </is>
+      </c>
+      <c r="B19" s="24" t="inlineStr">
         <is>
           <t>VIST</t>
         </is>
@@ -768,13 +1471,17 @@
           <t>VIST/CSAN</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="D19" s="25" t="n">
         <v>2.41</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n"/>
-      <c r="B20" s="1" t="inlineStr">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Energy</t>
+        </is>
+      </c>
+      <c r="B20" s="24" t="inlineStr">
         <is>
           <t>VIST</t>
         </is>
@@ -784,13 +1491,17 @@
           <t>VIST/EC</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="D20" s="26" t="n">
         <v>2.67</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n"/>
-      <c r="B21" s="1" t="inlineStr">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Energy</t>
+        </is>
+      </c>
+      <c r="B21" s="27" t="inlineStr">
         <is>
           <t>YPF</t>
         </is>
@@ -800,17 +1511,17 @@
           <t>YPF/CSAN</t>
         </is>
       </c>
-      <c r="D21" t="n">
+      <c r="D21" s="28" t="n">
         <v>2.59</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>Financials</t>
-        </is>
-      </c>
-      <c r="B22" s="1" t="inlineStr">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B22" s="29" t="inlineStr">
         <is>
           <t>BAP</t>
         </is>
@@ -820,13 +1531,17 @@
           <t>BAP/BBD</t>
         </is>
       </c>
-      <c r="D22" t="n">
+      <c r="D22" s="30" t="n">
         <v>3.43</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n"/>
-      <c r="B23" s="1" t="inlineStr">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B23" s="29" t="inlineStr">
         <is>
           <t>BAP</t>
         </is>
@@ -836,13 +1551,17 @@
           <t>BAP/BSBR</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="D23" s="6" t="n">
         <v>2.89</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n"/>
-      <c r="B24" s="1" t="inlineStr">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B24" s="29" t="inlineStr">
         <is>
           <t>BAP</t>
         </is>
@@ -852,13 +1571,17 @@
           <t>BAP/BCH</t>
         </is>
       </c>
-      <c r="D24" t="n">
+      <c r="D24" s="22" t="n">
         <v>2.61</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n"/>
-      <c r="B25" s="1" t="inlineStr">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B25" s="29" t="inlineStr">
         <is>
           <t>BAP</t>
         </is>
@@ -868,13 +1591,17 @@
           <t>BAP/BSAC</t>
         </is>
       </c>
-      <c r="D25" t="n">
+      <c r="D25" s="31" t="n">
         <v>3.16</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n"/>
-      <c r="B26" s="1" t="inlineStr">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B26" s="32" t="inlineStr">
         <is>
           <t>BBAR</t>
         </is>
@@ -884,13 +1611,17 @@
           <t>BBAR/BMA</t>
         </is>
       </c>
-      <c r="D26" t="n">
+      <c r="D26" s="33" t="n">
         <v>-2.18</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n"/>
-      <c r="B27" s="1" t="inlineStr">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B27" s="32" t="inlineStr">
         <is>
           <t>BBAR</t>
         </is>
@@ -900,13 +1631,17 @@
           <t>BBAR/BBD</t>
         </is>
       </c>
-      <c r="D27" t="n">
+      <c r="D27" s="34" t="n">
         <v>3.5</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n"/>
-      <c r="B28" s="1" t="inlineStr">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B28" s="32" t="inlineStr">
         <is>
           <t>BBAR</t>
         </is>
@@ -916,13 +1651,17 @@
           <t>BBAR/BSBR</t>
         </is>
       </c>
-      <c r="D28" t="n">
+      <c r="D28" s="16" t="n">
         <v>2.47</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="n"/>
-      <c r="B29" s="1" t="inlineStr">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B29" s="35" t="inlineStr">
         <is>
           <t>BBD</t>
         </is>
@@ -932,13 +1671,17 @@
           <t>BBD/BMA</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="D29" s="36" t="n">
         <v>-2.72</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n"/>
-      <c r="B30" s="1" t="inlineStr">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B30" s="35" t="inlineStr">
         <is>
           <t>BBD</t>
         </is>
@@ -948,13 +1691,17 @@
           <t>BBD/BBAR</t>
         </is>
       </c>
-      <c r="D30" t="n">
+      <c r="D30" s="37" t="n">
         <v>-2.7</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n"/>
-      <c r="B31" s="1" t="inlineStr">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B31" s="35" t="inlineStr">
         <is>
           <t>BBD</t>
         </is>
@@ -964,13 +1711,17 @@
           <t>BBD/GGAL</t>
         </is>
       </c>
-      <c r="D31" t="n">
+      <c r="D31" s="38" t="n">
         <v>-2.54</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n"/>
-      <c r="B32" s="1" t="inlineStr">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B32" s="35" t="inlineStr">
         <is>
           <t>BBD</t>
         </is>
@@ -980,13 +1731,17 @@
           <t>BBD/SUPV</t>
         </is>
       </c>
-      <c r="D32" t="n">
+      <c r="D32" s="39" t="n">
         <v>-2.08</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n"/>
-      <c r="B33" s="1" t="inlineStr">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B33" s="35" t="inlineStr">
         <is>
           <t>BBD</t>
         </is>
@@ -996,13 +1751,17 @@
           <t>BBD/ITUB</t>
         </is>
       </c>
-      <c r="D33" t="n">
+      <c r="D33" s="40" t="n">
         <v>-2.79</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="n"/>
-      <c r="B34" s="1" t="inlineStr">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B34" s="35" t="inlineStr">
         <is>
           <t>BBD</t>
         </is>
@@ -1012,13 +1771,17 @@
           <t>BBD/NU</t>
         </is>
       </c>
-      <c r="D34" t="n">
+      <c r="D34" s="19" t="n">
         <v>-2.05</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n"/>
-      <c r="B35" s="1" t="inlineStr">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B35" s="35" t="inlineStr">
         <is>
           <t>BBD</t>
         </is>
@@ -1028,13 +1791,17 @@
           <t>BBD/PAGS</t>
         </is>
       </c>
-      <c r="D35" t="n">
+      <c r="D35" s="41" t="n">
         <v>-2.29</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n"/>
-      <c r="B36" s="1" t="inlineStr">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B36" s="35" t="inlineStr">
         <is>
           <t>BBD</t>
         </is>
@@ -1044,13 +1811,17 @@
           <t>BBD/STNE</t>
         </is>
       </c>
-      <c r="D36" t="n">
+      <c r="D36" s="18" t="n">
         <v>-2.02</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n"/>
-      <c r="B37" s="1" t="inlineStr">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B37" s="35" t="inlineStr">
         <is>
           <t>BBD</t>
         </is>
@@ -1060,13 +1831,17 @@
           <t>BBD/CIB</t>
         </is>
       </c>
-      <c r="D37" t="n">
+      <c r="D37" s="3" t="n">
         <v>-2.59</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="n"/>
-      <c r="B38" s="1" t="inlineStr">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B38" s="35" t="inlineStr">
         <is>
           <t>BBD</t>
         </is>
@@ -1076,13 +1851,17 @@
           <t>BBD/BAP</t>
         </is>
       </c>
-      <c r="D38" t="n">
+      <c r="D38" s="42" t="n">
         <v>-2.78</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="n"/>
-      <c r="B39" s="1" t="inlineStr">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B39" s="43" t="inlineStr">
         <is>
           <t>BCH</t>
         </is>
@@ -1092,13 +1871,17 @@
           <t>BCH/BMA</t>
         </is>
       </c>
-      <c r="D39" t="n">
+      <c r="D39" s="13" t="n">
         <v>-2.12</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n"/>
-      <c r="B40" s="1" t="inlineStr">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B40" s="43" t="inlineStr">
         <is>
           <t>BCH</t>
         </is>
@@ -1108,13 +1891,17 @@
           <t>BCH/BAP</t>
         </is>
       </c>
-      <c r="D40" t="n">
+      <c r="D40" s="33" t="n">
         <v>-2.18</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="n"/>
-      <c r="B41" s="1" t="inlineStr">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B41" s="44" t="inlineStr">
         <is>
           <t>BMA</t>
         </is>
@@ -1124,13 +1911,17 @@
           <t>BMA/BBAR</t>
         </is>
       </c>
-      <c r="D41" t="n">
+      <c r="D41" s="16" t="n">
         <v>2.49</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="n"/>
-      <c r="B42" s="1" t="inlineStr">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B42" s="44" t="inlineStr">
         <is>
           <t>BMA</t>
         </is>
@@ -1140,13 +1931,17 @@
           <t>BMA/BBD</t>
         </is>
       </c>
-      <c r="D42" t="n">
+      <c r="D42" s="45" t="n">
         <v>4.02</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n"/>
-      <c r="B43" s="1" t="inlineStr">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B43" s="44" t="inlineStr">
         <is>
           <t>BMA</t>
         </is>
@@ -1156,13 +1951,17 @@
           <t>BMA/BSBR</t>
         </is>
       </c>
-      <c r="D43" t="n">
+      <c r="D43" s="46" t="n">
         <v>3.49</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="n"/>
-      <c r="B44" s="1" t="inlineStr">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B44" s="44" t="inlineStr">
         <is>
           <t>BMA</t>
         </is>
@@ -1172,13 +1971,17 @@
           <t>BMA/ITUB</t>
         </is>
       </c>
-      <c r="D44" t="n">
+      <c r="D44" s="47" t="n">
         <v>2.74</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="n"/>
-      <c r="B45" s="1" t="inlineStr">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B45" s="44" t="inlineStr">
         <is>
           <t>BMA</t>
         </is>
@@ -1188,13 +1991,17 @@
           <t>BMA/BCH</t>
         </is>
       </c>
-      <c r="D45" t="n">
+      <c r="D45" s="48" t="n">
         <v>3.05</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n"/>
-      <c r="B46" s="1" t="inlineStr">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B46" s="44" t="inlineStr">
         <is>
           <t>BMA</t>
         </is>
@@ -1204,13 +2011,17 @@
           <t>BMA/BSAC</t>
         </is>
       </c>
-      <c r="D46" t="n">
+      <c r="D46" s="49" t="n">
         <v>2.97</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n"/>
-      <c r="B47" s="1" t="inlineStr">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B47" s="44" t="inlineStr">
         <is>
           <t>BMA</t>
         </is>
@@ -1220,13 +2031,17 @@
           <t>BMA/CIB</t>
         </is>
       </c>
-      <c r="D47" t="n">
+      <c r="D47" s="23" t="n">
         <v>2.27</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="n"/>
-      <c r="B48" s="1" t="inlineStr">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B48" s="44" t="inlineStr">
         <is>
           <t>BMA</t>
         </is>
@@ -1236,13 +2051,17 @@
           <t>BMA/DLO</t>
         </is>
       </c>
-      <c r="D48" t="n">
+      <c r="D48" s="50" t="n">
         <v>2.1</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="n"/>
-      <c r="B49" s="1" t="inlineStr">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B49" s="51" t="inlineStr">
         <is>
           <t>BSAC</t>
         </is>
@@ -1252,13 +2071,17 @@
           <t>BSAC/BMA</t>
         </is>
       </c>
-      <c r="D49" t="n">
+      <c r="D49" s="52" t="n">
         <v>-2.14</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="n"/>
-      <c r="B50" s="1" t="inlineStr">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B50" s="51" t="inlineStr">
         <is>
           <t>BSAC</t>
         </is>
@@ -1268,13 +2091,17 @@
           <t>BSAC/CIB</t>
         </is>
       </c>
-      <c r="D50" t="n">
+      <c r="D50" s="13" t="n">
         <v>-2.1</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="n"/>
-      <c r="B51" s="1" t="inlineStr">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B51" s="51" t="inlineStr">
         <is>
           <t>BSAC</t>
         </is>
@@ -1284,13 +2111,17 @@
           <t>BSAC/BAP</t>
         </is>
       </c>
-      <c r="D51" t="n">
+      <c r="D51" s="53" t="n">
         <v>-2.65</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="n"/>
-      <c r="B52" s="1" t="inlineStr">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B52" s="54" t="inlineStr">
         <is>
           <t>BSBR</t>
         </is>
@@ -1300,13 +2131,17 @@
           <t>BSBR/BMA</t>
         </is>
       </c>
-      <c r="D52" t="n">
+      <c r="D52" s="55" t="n">
         <v>-2.39</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="n"/>
-      <c r="B53" s="1" t="inlineStr">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B53" s="54" t="inlineStr">
         <is>
           <t>BSBR</t>
         </is>
@@ -1316,13 +2151,17 @@
           <t>BSBR/BBAR</t>
         </is>
       </c>
-      <c r="D53" t="n">
+      <c r="D53" s="18" t="n">
         <v>-2.01</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="n"/>
-      <c r="B54" s="1" t="inlineStr">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B54" s="54" t="inlineStr">
         <is>
           <t>BSBR</t>
         </is>
@@ -1332,13 +2171,17 @@
           <t>BSBR/GGAL</t>
         </is>
       </c>
-      <c r="D54" t="n">
+      <c r="D54" s="13" t="n">
         <v>-2.11</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="n"/>
-      <c r="B55" s="1" t="inlineStr">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B55" s="54" t="inlineStr">
         <is>
           <t>BSBR</t>
         </is>
@@ -1348,13 +2191,17 @@
           <t>BSBR/ITUB</t>
         </is>
       </c>
-      <c r="D55" t="n">
+      <c r="D55" s="55" t="n">
         <v>-2.4</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="n"/>
-      <c r="B56" s="1" t="inlineStr">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B56" s="54" t="inlineStr">
         <is>
           <t>BSBR</t>
         </is>
@@ -1364,13 +2211,17 @@
           <t>BSBR/PAGS</t>
         </is>
       </c>
-      <c r="D56" t="n">
+      <c r="D56" s="18" t="n">
         <v>-2.01</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="n"/>
-      <c r="B57" s="1" t="inlineStr">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B57" s="54" t="inlineStr">
         <is>
           <t>BSBR</t>
         </is>
@@ -1380,13 +2231,17 @@
           <t>BSBR/CIB</t>
         </is>
       </c>
-      <c r="D57" t="n">
+      <c r="D57" s="12" t="n">
         <v>-2.27</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="n"/>
-      <c r="B58" s="1" t="inlineStr">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B58" s="54" t="inlineStr">
         <is>
           <t>BSBR</t>
         </is>
@@ -1396,13 +2251,17 @@
           <t>BSBR/BAP</t>
         </is>
       </c>
-      <c r="D58" t="n">
+      <c r="D58" s="41" t="n">
         <v>-2.3</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="n"/>
-      <c r="B59" s="1" t="inlineStr">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B59" s="56" t="inlineStr">
         <is>
           <t>CIB</t>
         </is>
@@ -1412,13 +2271,17 @@
           <t>CIB/BBD</t>
         </is>
       </c>
-      <c r="D59" t="n">
+      <c r="D59" s="57" t="n">
         <v>3.19</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="n"/>
-      <c r="B60" s="1" t="inlineStr">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B60" s="56" t="inlineStr">
         <is>
           <t>CIB</t>
         </is>
@@ -1428,13 +2291,17 @@
           <t>CIB/BSBR</t>
         </is>
       </c>
-      <c r="D60" t="n">
+      <c r="D60" s="58" t="n">
         <v>2.76</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="n"/>
-      <c r="B61" s="1" t="inlineStr">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B61" s="56" t="inlineStr">
         <is>
           <t>CIB</t>
         </is>
@@ -1444,13 +2311,17 @@
           <t>CIB/BCH</t>
         </is>
       </c>
-      <c r="D61" t="n">
+      <c r="D61" s="23" t="n">
         <v>2.25</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="n"/>
-      <c r="B62" s="1" t="inlineStr">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B62" s="56" t="inlineStr">
         <is>
           <t>CIB</t>
         </is>
@@ -1460,13 +2331,17 @@
           <t>CIB/BSAC</t>
         </is>
       </c>
-      <c r="D62" t="n">
+      <c r="D62" s="59" t="n">
         <v>2.36</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="n"/>
-      <c r="B63" s="1" t="inlineStr">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B63" s="60" t="inlineStr">
         <is>
           <t>GGAL</t>
         </is>
@@ -1476,13 +2351,17 @@
           <t>GGAL/BBAR</t>
         </is>
       </c>
-      <c r="D63" t="n">
+      <c r="D63" s="10" t="n">
         <v>2.07</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="n"/>
-      <c r="B64" s="1" t="inlineStr">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B64" s="60" t="inlineStr">
         <is>
           <t>GGAL</t>
         </is>
@@ -1492,13 +2371,17 @@
           <t>GGAL/BBD</t>
         </is>
       </c>
-      <c r="D64" t="n">
+      <c r="D64" s="34" t="n">
         <v>3.53</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="n"/>
-      <c r="B65" s="1" t="inlineStr">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B65" s="60" t="inlineStr">
         <is>
           <t>GGAL</t>
         </is>
@@ -1508,13 +2391,17 @@
           <t>GGAL/BSBR</t>
         </is>
       </c>
-      <c r="D65" t="n">
+      <c r="D65" s="6" t="n">
         <v>2.9</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="n"/>
-      <c r="B66" s="1" t="inlineStr">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B66" s="60" t="inlineStr">
         <is>
           <t>GGAL</t>
         </is>
@@ -1524,13 +2411,17 @@
           <t>GGAL/BCH</t>
         </is>
       </c>
-      <c r="D66" t="n">
+      <c r="D66" s="61" t="n">
         <v>2.52</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="n"/>
-      <c r="B67" s="1" t="inlineStr">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B67" s="60" t="inlineStr">
         <is>
           <t>GGAL</t>
         </is>
@@ -1540,13 +2431,17 @@
           <t>GGAL/BSAC</t>
         </is>
       </c>
-      <c r="D67" t="n">
+      <c r="D67" s="62" t="n">
         <v>2.55</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="n"/>
-      <c r="B68" s="1" t="inlineStr">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B68" s="63" t="inlineStr">
         <is>
           <t>ITUB</t>
         </is>
@@ -1556,13 +2451,17 @@
           <t>ITUB/BMA</t>
         </is>
       </c>
-      <c r="D68" t="n">
+      <c r="D68" s="52" t="n">
         <v>-2.14</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="n"/>
-      <c r="B69" s="1" t="inlineStr">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B69" s="63" t="inlineStr">
         <is>
           <t>ITUB</t>
         </is>
@@ -1572,13 +2471,17 @@
           <t>ITUB/BBD</t>
         </is>
       </c>
-      <c r="D69" t="n">
+      <c r="D69" s="64" t="n">
         <v>3.12</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="n"/>
-      <c r="B70" s="1" t="inlineStr">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B70" s="63" t="inlineStr">
         <is>
           <t>ITUB</t>
         </is>
@@ -1588,13 +2491,17 @@
           <t>ITUB/BSBR</t>
         </is>
       </c>
-      <c r="D70" t="n">
+      <c r="D70" s="47" t="n">
         <v>2.72</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="n"/>
-      <c r="B71" s="1" t="inlineStr">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B71" s="65" t="inlineStr">
         <is>
           <t>NU</t>
         </is>
@@ -1604,13 +2511,17 @@
           <t>NU/BBD</t>
         </is>
       </c>
-      <c r="D71" t="n">
+      <c r="D71" s="66" t="n">
         <v>2.87</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="n"/>
-      <c r="B72" s="1" t="inlineStr">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B72" s="65" t="inlineStr">
         <is>
           <t>NU</t>
         </is>
@@ -1620,13 +2531,17 @@
           <t>NU/BSBR</t>
         </is>
       </c>
-      <c r="D72" t="n">
+      <c r="D72" s="59" t="n">
         <v>2.37</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="n"/>
-      <c r="B73" s="1" t="inlineStr">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B73" s="67" t="inlineStr">
         <is>
           <t>PAGS</t>
         </is>
@@ -1636,13 +2551,17 @@
           <t>PAGS/BBD</t>
         </is>
       </c>
-      <c r="D73" t="n">
+      <c r="D73" s="68" t="n">
         <v>2.81</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="n"/>
-      <c r="B74" s="1" t="inlineStr">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B74" s="67" t="inlineStr">
         <is>
           <t>PAGS</t>
         </is>
@@ -1652,13 +2571,17 @@
           <t>PAGS/BSBR</t>
         </is>
       </c>
-      <c r="D74" t="n">
+      <c r="D74" s="25" t="n">
         <v>2.43</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="n"/>
-      <c r="B75" s="1" t="inlineStr">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B75" s="69" t="inlineStr">
         <is>
           <t>STNE</t>
         </is>
@@ -1668,13 +2591,17 @@
           <t>STNE/BBD</t>
         </is>
       </c>
-      <c r="D75" t="n">
+      <c r="D75" s="59" t="n">
         <v>2.36</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="n"/>
-      <c r="B76" s="1" t="inlineStr">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B76" s="70" t="inlineStr">
         <is>
           <t>SUPV</t>
         </is>
@@ -1684,13 +2611,17 @@
           <t>SUPV/BBD</t>
         </is>
       </c>
-      <c r="D76" t="n">
+      <c r="D76" s="6" t="n">
         <v>2.89</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="n"/>
-      <c r="B77" s="1" t="inlineStr">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B77" s="70" t="inlineStr">
         <is>
           <t>SUPV</t>
         </is>
@@ -1700,13 +2631,17 @@
           <t>SUPV/BSBR</t>
         </is>
       </c>
-      <c r="D77" t="n">
+      <c r="D77" s="16" t="n">
         <v>2.49</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="n"/>
-      <c r="B78" s="1" t="inlineStr">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B78" s="70" t="inlineStr">
         <is>
           <t>SUPV</t>
         </is>
@@ -1716,13 +2651,17 @@
           <t>SUPV/BCH</t>
         </is>
       </c>
-      <c r="D78" t="n">
+      <c r="D78" s="71" t="n">
         <v>2.14</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="n"/>
-      <c r="B79" s="1" t="inlineStr">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B79" s="70" t="inlineStr">
         <is>
           <t>SUPV</t>
         </is>
@@ -1732,17 +2671,17 @@
           <t>SUPV/BSAC</t>
         </is>
       </c>
-      <c r="D79" t="n">
+      <c r="D79" s="10" t="n">
         <v>2.08</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="inlineStr">
+      <c r="A80" t="inlineStr">
         <is>
           <t>Industrials</t>
         </is>
       </c>
-      <c r="B80" s="1" t="inlineStr">
+      <c r="B80" s="72" t="inlineStr">
         <is>
           <t>ASR</t>
         </is>
@@ -1752,13 +2691,17 @@
           <t>ASR/GOL</t>
         </is>
       </c>
-      <c r="D80" t="n">
+      <c r="D80" s="73" t="n">
         <v>3.38</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1" t="n"/>
-      <c r="B81" s="1" t="inlineStr">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B81" s="72" t="inlineStr">
         <is>
           <t>ASR</t>
         </is>
@@ -1768,13 +2711,17 @@
           <t>ASR/OMAB</t>
         </is>
       </c>
-      <c r="D81" t="n">
+      <c r="D81" s="16" t="n">
         <v>2.48</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="n"/>
-      <c r="B82" s="1" t="inlineStr">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B82" s="72" t="inlineStr">
         <is>
           <t>ASR</t>
         </is>
@@ -1784,13 +2731,17 @@
           <t>ASR/PAC</t>
         </is>
       </c>
-      <c r="D82" t="n">
+      <c r="D82" s="28" t="n">
         <v>2.57</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="n"/>
-      <c r="B83" s="1" t="inlineStr">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B83" s="74" t="inlineStr">
         <is>
           <t>AZUL</t>
         </is>
@@ -1800,13 +2751,17 @@
           <t>AZUL/GOL</t>
         </is>
       </c>
-      <c r="D83" t="n">
+      <c r="D83" s="75" t="n">
         <v>3.15</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="1" t="n"/>
-      <c r="B84" s="1" t="inlineStr">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B84" s="76" t="inlineStr">
         <is>
           <t>ERJ</t>
         </is>
@@ -1816,13 +2771,17 @@
           <t>ERJ/AZUL</t>
         </is>
       </c>
-      <c r="D84" t="n">
+      <c r="D84" s="8" t="n">
         <v>2.03</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="1" t="n"/>
-      <c r="B85" s="1" t="inlineStr">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B85" s="76" t="inlineStr">
         <is>
           <t>ERJ</t>
         </is>
@@ -1832,13 +2791,17 @@
           <t>ERJ/GOL</t>
         </is>
       </c>
-      <c r="D85" t="n">
+      <c r="D85" s="77" t="n">
         <v>3.56</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="1" t="n"/>
-      <c r="B86" s="1" t="inlineStr">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B86" s="78" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
@@ -1848,13 +2811,17 @@
           <t>GOL/AZUL</t>
         </is>
       </c>
-      <c r="D86" t="n">
+      <c r="D86" s="79" t="n">
         <v>-3.07</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="1" t="n"/>
-      <c r="B87" s="1" t="inlineStr">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B87" s="78" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
@@ -1864,13 +2831,17 @@
           <t>GOL/ERJ</t>
         </is>
       </c>
-      <c r="D87" t="n">
+      <c r="D87" s="80" t="n">
         <v>-2.32</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="1" t="n"/>
-      <c r="B88" s="1" t="inlineStr">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B88" s="78" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
@@ -1880,13 +2851,17 @@
           <t>GOL/TGLS</t>
         </is>
       </c>
-      <c r="D88" t="n">
+      <c r="D88" s="3" t="n">
         <v>-2.57</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="1" t="n"/>
-      <c r="B89" s="1" t="inlineStr">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B89" s="78" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
@@ -1896,13 +2871,17 @@
           <t>GOL/OMAB</t>
         </is>
       </c>
-      <c r="D89" t="n">
+      <c r="D89" s="19" t="n">
         <v>-2.05</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="1" t="n"/>
-      <c r="B90" s="1" t="inlineStr">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B90" s="78" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
@@ -1912,13 +2891,17 @@
           <t>GOL/PAC</t>
         </is>
       </c>
-      <c r="D90" t="n">
+      <c r="D90" s="13" t="n">
         <v>-2.12</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="1" t="n"/>
-      <c r="B91" s="1" t="inlineStr">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B91" s="78" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
@@ -1928,13 +2911,17 @@
           <t>GOL/ASR</t>
         </is>
       </c>
-      <c r="D91" t="n">
+      <c r="D91" s="41" t="n">
         <v>-2.3</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="1" t="n"/>
-      <c r="B92" s="1" t="inlineStr">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B92" s="81" t="inlineStr">
         <is>
           <t>OMAB</t>
         </is>
@@ -1944,13 +2931,17 @@
           <t>OMAB/GOL</t>
         </is>
       </c>
-      <c r="D92" t="n">
+      <c r="D92" s="48" t="n">
         <v>3.04</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="1" t="n"/>
-      <c r="B93" s="1" t="inlineStr">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B93" s="81" t="inlineStr">
         <is>
           <t>OMAB</t>
         </is>
@@ -1960,13 +2951,17 @@
           <t>OMAB/ASR</t>
         </is>
       </c>
-      <c r="D93" t="n">
+      <c r="D93" s="19" t="n">
         <v>-2.04</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="1" t="n"/>
-      <c r="B94" s="1" t="inlineStr">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B94" s="82" t="inlineStr">
         <is>
           <t>PAC</t>
         </is>
@@ -1976,13 +2971,17 @@
           <t>PAC/GOL</t>
         </is>
       </c>
-      <c r="D94" t="n">
+      <c r="D94" s="64" t="n">
         <v>3.1</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="1" t="n"/>
-      <c r="B95" s="1" t="inlineStr">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B95" s="82" t="inlineStr">
         <is>
           <t>PAC</t>
         </is>
@@ -1992,13 +2991,17 @@
           <t>PAC/ASR</t>
         </is>
       </c>
-      <c r="D95" t="n">
+      <c r="D95" s="80" t="n">
         <v>-2.34</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="1" t="n"/>
-      <c r="B96" s="1" t="inlineStr">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B96" s="83" t="inlineStr">
         <is>
           <t>TGLS</t>
         </is>
@@ -2008,13 +3011,17 @@
           <t>TGLS/GOL</t>
         </is>
       </c>
-      <c r="D96" t="n">
+      <c r="D96" s="46" t="n">
         <v>3.48</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="1" t="n"/>
-      <c r="B97" s="1" t="inlineStr">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B97" s="83" t="inlineStr">
         <is>
           <t>TGLS</t>
         </is>
@@ -2024,13 +3031,17 @@
           <t>TGLS/VLRS</t>
         </is>
       </c>
-      <c r="D97" t="n">
+      <c r="D97" s="10" t="n">
         <v>2.07</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="1" t="n"/>
-      <c r="B98" s="1" t="inlineStr">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B98" s="84" t="inlineStr">
         <is>
           <t>VLRS</t>
         </is>
@@ -2040,17 +3051,17 @@
           <t>VLRS/GOL</t>
         </is>
       </c>
-      <c r="D98" t="n">
+      <c r="D98" s="85" t="n">
         <v>2.7</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="1" t="inlineStr">
+      <c r="A99" t="inlineStr">
         <is>
           <t>Materials</t>
         </is>
       </c>
-      <c r="B99" s="1" t="inlineStr">
+      <c r="B99" s="86" t="inlineStr">
         <is>
           <t>ALB</t>
         </is>
@@ -2060,13 +3071,17 @@
           <t>ALB/SGML</t>
         </is>
       </c>
-      <c r="D99" t="n">
+      <c r="D99" s="45" t="n">
         <v>5.49</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="1" t="n"/>
-      <c r="B100" s="1" t="inlineStr">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B100" s="87" t="inlineStr">
         <is>
           <t>BAK</t>
         </is>
@@ -2076,13 +3091,17 @@
           <t>BAK/SGML</t>
         </is>
       </c>
-      <c r="D100" t="n">
+      <c r="D100" s="45" t="n">
         <v>5.96</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="1" t="n"/>
-      <c r="B101" s="1" t="inlineStr">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B101" s="87" t="inlineStr">
         <is>
           <t>BAK</t>
         </is>
@@ -2092,13 +3111,17 @@
           <t>BAK/SQM</t>
         </is>
       </c>
-      <c r="D101" t="n">
+      <c r="D101" s="10" t="n">
         <v>2.08</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="1" t="n"/>
-      <c r="B102" s="1" t="inlineStr">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B102" s="88" t="inlineStr">
         <is>
           <t>BVN</t>
         </is>
@@ -2108,13 +3131,17 @@
           <t>BVN/LOMA</t>
         </is>
       </c>
-      <c r="D102" t="n">
+      <c r="D102" s="89" t="n">
         <v>2.19</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="1" t="n"/>
-      <c r="B103" s="1" t="inlineStr">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B103" s="88" t="inlineStr">
         <is>
           <t>BVN</t>
         </is>
@@ -2124,13 +3151,17 @@
           <t>BVN/SID</t>
         </is>
       </c>
-      <c r="D103" t="n">
+      <c r="D103" s="71" t="n">
         <v>2.15</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="1" t="n"/>
-      <c r="B104" s="1" t="inlineStr">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B104" s="88" t="inlineStr">
         <is>
           <t>BVN</t>
         </is>
@@ -2140,13 +3171,17 @@
           <t>BVN/GGB</t>
         </is>
       </c>
-      <c r="D104" t="n">
+      <c r="D104" s="90" t="n">
         <v>2.3</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="1" t="n"/>
-      <c r="B105" s="1" t="inlineStr">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B105" s="88" t="inlineStr">
         <is>
           <t>BVN</t>
         </is>
@@ -2156,13 +3191,17 @@
           <t>BVN/VALE</t>
         </is>
       </c>
-      <c r="D105" t="n">
+      <c r="D105" s="16" t="n">
         <v>2.49</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="1" t="n"/>
-      <c r="B106" s="1" t="inlineStr">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B106" s="88" t="inlineStr">
         <is>
           <t>BVN</t>
         </is>
@@ -2172,13 +3211,17 @@
           <t>BVN/SGML</t>
         </is>
       </c>
-      <c r="D106" t="n">
+      <c r="D106" s="45" t="n">
         <v>4.5</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="1" t="n"/>
-      <c r="B107" s="1" t="inlineStr">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B107" s="88" t="inlineStr">
         <is>
           <t>BVN</t>
         </is>
@@ -2188,13 +3231,17 @@
           <t>BVN/SQM</t>
         </is>
       </c>
-      <c r="D107" t="n">
+      <c r="D107" s="91" t="n">
         <v>2.39</v>
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="1" t="n"/>
-      <c r="B108" s="1" t="inlineStr">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B108" s="88" t="inlineStr">
         <is>
           <t>BVN</t>
         </is>
@@ -2204,13 +3251,17 @@
           <t>BVN/ALB</t>
         </is>
       </c>
-      <c r="D108" t="n">
+      <c r="D108" s="5" t="n">
         <v>2.16</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="1" t="n"/>
-      <c r="B109" s="1" t="inlineStr">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B109" s="92" t="inlineStr">
         <is>
           <t>CX</t>
         </is>
@@ -2220,13 +3271,17 @@
           <t>CX/GGB</t>
         </is>
       </c>
-      <c r="D109" t="n">
+      <c r="D109" s="5" t="n">
         <v>2.16</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="1" t="n"/>
-      <c r="B110" s="1" t="inlineStr">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B110" s="92" t="inlineStr">
         <is>
           <t>CX</t>
         </is>
@@ -2236,13 +3291,17 @@
           <t>CX/SGML</t>
         </is>
       </c>
-      <c r="D110" t="n">
+      <c r="D110" s="45" t="n">
         <v>4.75</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="1" t="n"/>
-      <c r="B111" s="1" t="inlineStr">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B111" s="92" t="inlineStr">
         <is>
           <t>CX</t>
         </is>
@@ -2252,13 +3311,17 @@
           <t>CX/SQM</t>
         </is>
       </c>
-      <c r="D111" t="n">
+      <c r="D111" s="50" t="n">
         <v>2.12</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="1" t="n"/>
-      <c r="B112" s="1" t="inlineStr">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B112" s="93" t="inlineStr">
         <is>
           <t>GGB</t>
         </is>
@@ -2268,13 +3331,17 @@
           <t>GGB/SGML</t>
         </is>
       </c>
-      <c r="D112" t="n">
+      <c r="D112" s="45" t="n">
         <v>5.11</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="1" t="n"/>
-      <c r="B113" s="1" t="inlineStr">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B113" s="94" t="inlineStr">
         <is>
           <t>LOMA</t>
         </is>
@@ -2284,13 +3351,17 @@
           <t>LOMA/SGML</t>
         </is>
       </c>
-      <c r="D113" t="n">
+      <c r="D113" s="45" t="n">
         <v>5.03</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="1" t="n"/>
-      <c r="B114" s="1" t="inlineStr">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B114" s="94" t="inlineStr">
         <is>
           <t>LOMA</t>
         </is>
@@ -2300,13 +3371,17 @@
           <t>LOMA/SQM</t>
         </is>
       </c>
-      <c r="D114" t="n">
+      <c r="D114" s="95" t="n">
         <v>2.06</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="1" t="n"/>
-      <c r="B115" s="1" t="inlineStr">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B115" s="96" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
@@ -2316,13 +3391,17 @@
           <t>SGML/LOMA</t>
         </is>
       </c>
-      <c r="D115" t="n">
+      <c r="D115" s="97" t="n">
         <v>-2.98</v>
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="1" t="n"/>
-      <c r="B116" s="1" t="inlineStr">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B116" s="96" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
@@ -2332,13 +3411,17 @@
           <t>SGML/SID</t>
         </is>
       </c>
-      <c r="D116" t="n">
+      <c r="D116" s="98" t="n">
         <v>-2.52</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="1" t="n"/>
-      <c r="B117" s="1" t="inlineStr">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B117" s="96" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
@@ -2348,13 +3431,17 @@
           <t>SGML/GGB</t>
         </is>
       </c>
-      <c r="D117" t="n">
+      <c r="D117" s="99" t="n">
         <v>-3.34</v>
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="1" t="n"/>
-      <c r="B118" s="1" t="inlineStr">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B118" s="96" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
@@ -2364,13 +3451,17 @@
           <t>SGML/SUZ</t>
         </is>
       </c>
-      <c r="D118" t="n">
+      <c r="D118" s="55" t="n">
         <v>-2.39</v>
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="1" t="n"/>
-      <c r="B119" s="1" t="inlineStr">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B119" s="96" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
@@ -2380,13 +3471,17 @@
           <t>SGML/BAK</t>
         </is>
       </c>
-      <c r="D119" t="n">
+      <c r="D119" s="100" t="n">
         <v>-3.4</v>
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="1" t="n"/>
-      <c r="B120" s="1" t="inlineStr">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B120" s="96" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
@@ -2396,13 +3491,17 @@
           <t>SGML/VALE</t>
         </is>
       </c>
-      <c r="D120" t="n">
+      <c r="D120" s="42" t="n">
         <v>-2.78</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="1" t="n"/>
-      <c r="B121" s="1" t="inlineStr">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B121" s="96" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
@@ -2412,13 +3511,17 @@
           <t>SGML/SQM</t>
         </is>
       </c>
-      <c r="D121" t="n">
+      <c r="D121" s="101" t="n">
         <v>-4.08</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="1" t="n"/>
-      <c r="B122" s="1" t="inlineStr">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B122" s="96" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
@@ -2428,13 +3531,17 @@
           <t>SGML/CX</t>
         </is>
       </c>
-      <c r="D122" t="n">
+      <c r="D122" s="98" t="n">
         <v>-2.51</v>
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="1" t="n"/>
-      <c r="B123" s="1" t="inlineStr">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B123" s="96" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
@@ -2444,13 +3551,17 @@
           <t>SGML/BVN</t>
         </is>
       </c>
-      <c r="D123" t="n">
+      <c r="D123" s="102" t="n">
         <v>-2.19</v>
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="1" t="n"/>
-      <c r="B124" s="1" t="inlineStr">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B124" s="96" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
@@ -2460,13 +3571,17 @@
           <t>SGML/ALB</t>
         </is>
       </c>
-      <c r="D124" t="n">
+      <c r="D124" s="103" t="n">
         <v>-3.45</v>
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="1" t="n"/>
-      <c r="B125" s="1" t="inlineStr">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B125" s="104" t="inlineStr">
         <is>
           <t>SID</t>
         </is>
@@ -2476,13 +3591,17 @@
           <t>SID/SGML</t>
         </is>
       </c>
-      <c r="D125" t="n">
+      <c r="D125" s="45" t="n">
         <v>4.44</v>
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="1" t="n"/>
-      <c r="B126" s="1" t="inlineStr">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B126" s="105" t="inlineStr">
         <is>
           <t>SQM</t>
         </is>
@@ -2492,13 +3611,17 @@
           <t>SQM/SGML</t>
         </is>
       </c>
-      <c r="D126" t="n">
+      <c r="D126" s="45" t="n">
         <v>6.09</v>
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="1" t="n"/>
-      <c r="B127" s="1" t="inlineStr">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B127" s="106" t="inlineStr">
         <is>
           <t>SUZ</t>
         </is>
@@ -2508,13 +3631,17 @@
           <t>SUZ/SGML</t>
         </is>
       </c>
-      <c r="D127" t="n">
+      <c r="D127" s="45" t="n">
         <v>4.7</v>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="1" t="n"/>
-      <c r="B128" s="1" t="inlineStr">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B128" s="107" t="inlineStr">
         <is>
           <t>VALE</t>
         </is>
@@ -2524,13 +3651,17 @@
           <t>VALE/SGML</t>
         </is>
       </c>
-      <c r="D128" t="n">
+      <c r="D128" s="45" t="n">
         <v>4.77</v>
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="1" t="n"/>
-      <c r="B129" s="1" t="inlineStr">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B129" s="107" t="inlineStr">
         <is>
           <t>VALE</t>
         </is>
@@ -2540,17 +3671,17 @@
           <t>VALE/BVN</t>
         </is>
       </c>
-      <c r="D129" t="n">
+      <c r="D129" s="13" t="n">
         <v>-2.11</v>
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="1" t="inlineStr">
+      <c r="A130" t="inlineStr">
         <is>
           <t>Utilities</t>
         </is>
       </c>
-      <c r="B130" s="1" t="inlineStr">
+      <c r="B130" s="108" t="inlineStr">
         <is>
           <t>EBR</t>
         </is>
@@ -2560,13 +3691,17 @@
           <t>EBR/ENIC</t>
         </is>
       </c>
-      <c r="D130" t="n">
+      <c r="D130" s="71" t="n">
         <v>2.14</v>
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="1" t="n"/>
-      <c r="B131" s="1" t="inlineStr">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Utilities</t>
+        </is>
+      </c>
+      <c r="B131" s="109" t="inlineStr">
         <is>
           <t>ELP</t>
         </is>
@@ -2576,13 +3711,17 @@
           <t>ELP/SBS</t>
         </is>
       </c>
-      <c r="D131" t="n">
+      <c r="D131" s="102" t="n">
         <v>-2.21</v>
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="1" t="n"/>
-      <c r="B132" s="1" t="inlineStr">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Utilities</t>
+        </is>
+      </c>
+      <c r="B132" s="110" t="inlineStr">
         <is>
           <t>SBS</t>
         </is>
@@ -2592,13 +3731,17 @@
           <t>SBS/PAM</t>
         </is>
       </c>
-      <c r="D132" t="n">
+      <c r="D132" s="8" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="1" t="n"/>
-      <c r="B133" s="1" t="inlineStr">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Utilities</t>
+        </is>
+      </c>
+      <c r="B133" s="110" t="inlineStr">
         <is>
           <t>SBS</t>
         </is>
@@ -2608,13 +3751,17 @@
           <t>SBS/CIG</t>
         </is>
       </c>
-      <c r="D133" t="n">
+      <c r="D133" s="8" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="1" t="n"/>
-      <c r="B134" s="1" t="inlineStr">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Utilities</t>
+        </is>
+      </c>
+      <c r="B134" s="110" t="inlineStr">
         <is>
           <t>SBS</t>
         </is>
@@ -2624,13 +3771,17 @@
           <t>SBS/ELP</t>
         </is>
       </c>
-      <c r="D134" t="n">
+      <c r="D134" s="25" t="n">
         <v>2.42</v>
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="1" t="n"/>
-      <c r="B135" s="1" t="inlineStr">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Utilities</t>
+        </is>
+      </c>
+      <c r="B135" s="110" t="inlineStr">
         <is>
           <t>SBS</t>
         </is>
@@ -2640,19 +3791,11 @@
           <t>SBS/ENIC</t>
         </is>
       </c>
-      <c r="D135" t="n">
+      <c r="D135" s="15" t="n">
         <v>2.22</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="A22:A79"/>
-    <mergeCell ref="A80:A98"/>
-    <mergeCell ref="A99:A129"/>
-    <mergeCell ref="A130:A135"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>